<commit_message>
New data with fewer pruned bundles
</commit_message>
<xml_diff>
--- a/outputs-card-400-families.xlsx
+++ b/outputs-card-400-families.xlsx
@@ -49182,22 +49182,22 @@
         <v>113</v>
       </c>
       <c r="AI3" t="n">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="AJ3" t="n">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="AK3" t="n">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="AL3" t="n">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="AM3" t="n">
-        <v>119</v>
+        <v>59</v>
       </c>
       <c r="AN3" t="n">
-        <v>114</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
@@ -49297,22 +49297,22 @@
         <v>314</v>
       </c>
       <c r="AI4" t="n">
-        <v>281</v>
+        <v>159</v>
       </c>
       <c r="AJ4" t="n">
-        <v>348</v>
+        <v>184</v>
       </c>
       <c r="AK4" t="n">
-        <v>329</v>
+        <v>166</v>
       </c>
       <c r="AL4" t="n">
-        <v>343</v>
+        <v>176</v>
       </c>
       <c r="AM4" t="n">
-        <v>292</v>
+        <v>150</v>
       </c>
       <c r="AN4" t="n">
-        <v>311</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
@@ -49412,19 +49412,19 @@
         <v>15</v>
       </c>
       <c r="AI6" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="n">
         <v>0</v>
       </c>
       <c r="AK6" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AL6" t="n">
         <v>0</v>
       </c>
       <c r="AM6" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AN6" t="n">
         <v>0</v>
@@ -49527,22 +49527,22 @@
         <v>28</v>
       </c>
       <c r="AI7" t="n">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="AJ7" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="AK7" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="AL7" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="AM7" t="n">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AN7" t="n">
-        <v>69</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
@@ -49642,22 +49642,22 @@
         <v>42</v>
       </c>
       <c r="AI8" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="AJ8" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="AK8" t="n">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="AL8" t="n">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="AM8" t="n">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="AN8" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -49757,22 +49757,22 @@
         <v>23</v>
       </c>
       <c r="AI9" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AJ9" t="n">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="AK9" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="AL9" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="AM9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AN9" t="n">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -49872,22 +49872,22 @@
         <v>5</v>
       </c>
       <c r="AI10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AJ10" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="AK10" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AL10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AM10" t="n">
         <v>3</v>
       </c>
       <c r="AN10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -49949,7 +49949,7 @@
         <v>116</v>
       </c>
       <c r="J14" t="n">
-        <v>114</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -49974,7 +49974,7 @@
         <v>302</v>
       </c>
       <c r="J15" t="n">
-        <v>317</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16">
@@ -49999,7 +49999,7 @@
         <v>17</v>
       </c>
       <c r="J16" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -50024,7 +50024,7 @@
         <v>39</v>
       </c>
       <c r="J17" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18">
@@ -50049,7 +50049,7 @@
         <v>36</v>
       </c>
       <c r="J18" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -50074,7 +50074,7 @@
         <v>18</v>
       </c>
       <c r="J19" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -50099,7 +50099,7 @@
         <v>6</v>
       </c>
       <c r="J20" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -50131,7 +50131,7 @@
         <v>106</v>
       </c>
       <c r="J23" t="n">
-        <v>118</v>
+        <v>338</v>
       </c>
     </row>
     <row r="24">
@@ -50156,7 +50156,7 @@
         <v>294</v>
       </c>
       <c r="J24" t="n">
-        <v>282</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -50288,7 +50288,7 @@
         <v>266</v>
       </c>
       <c r="J32" t="n">
-        <v>176</v>
+        <v>976</v>
       </c>
     </row>
     <row r="33">
@@ -50313,7 +50313,7 @@
         <v>774</v>
       </c>
       <c r="J33" t="n">
-        <v>864</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -50774,7 +50774,7 @@
         <v>326</v>
       </c>
       <c r="J19" t="n">
-        <v>72</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20">
@@ -50799,7 +50799,7 @@
         <v>246</v>
       </c>
       <c r="J20" t="n">
-        <v>156</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -50824,7 +50824,7 @@
         <v>76</v>
       </c>
       <c r="J21" t="n">
-        <v>141</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
@@ -50849,7 +50849,7 @@
         <v>25</v>
       </c>
       <c r="J22" t="n">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
@@ -50874,7 +50874,7 @@
         <v>18</v>
       </c>
       <c r="J23" t="n">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24">
@@ -50899,7 +50899,7 @@
         <v>3</v>
       </c>
       <c r="J24" t="n">
-        <v>189</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
@@ -50931,7 +50931,7 @@
         <v>874</v>
       </c>
       <c r="J28" t="n">
-        <v>205</v>
+        <v>403</v>
       </c>
     </row>
     <row r="29">
@@ -50956,7 +50956,7 @@
         <v>655</v>
       </c>
       <c r="J29" t="n">
-        <v>478</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30">
@@ -50981,7 +50981,7 @@
         <v>183</v>
       </c>
       <c r="J30" t="n">
-        <v>391</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31">
@@ -51006,7 +51006,7 @@
         <v>57</v>
       </c>
       <c r="J31" t="n">
-        <v>158</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32">
@@ -51031,7 +51031,7 @@
         <v>38</v>
       </c>
       <c r="J32" t="n">
-        <v>201</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33">
@@ -51056,7 +51056,7 @@
         <v>7</v>
       </c>
       <c r="J33" t="n">
-        <v>471</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36">
@@ -51124,7 +51124,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>121</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -51144,7 +51144,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -51164,7 +51164,7 @@
         <v>188</v>
       </c>
       <c r="G4" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -51184,7 +51184,7 @@
         <v>32</v>
       </c>
       <c r="G5" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -51204,7 +51204,7 @@
         <v>6</v>
       </c>
       <c r="G6" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -51244,7 +51244,7 @@
         <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -51264,7 +51264,7 @@
         <v>3</v>
       </c>
       <c r="G9" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -51284,7 +51284,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -51344,7 +51344,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -51384,7 +51384,7 @@
         <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -51404,7 +51404,7 @@
         <v>3</v>
       </c>
       <c r="G16" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -51424,7 +51424,7 @@
         <v>38</v>
       </c>
       <c r="G17" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -51444,7 +51444,7 @@
         <v>18</v>
       </c>
       <c r="G18" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -51464,7 +51464,7 @@
         <v>41</v>
       </c>
       <c r="G19" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -51484,7 +51484,7 @@
         <v>9</v>
       </c>
       <c r="G20" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -51584,7 +51584,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -51604,7 +51604,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>0</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27">
@@ -51624,7 +51624,7 @@
         <v>57</v>
       </c>
       <c r="G27" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -51664,7 +51664,7 @@
         <v>35</v>
       </c>
       <c r="G29" t="n">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30">
@@ -51684,7 +51684,7 @@
         <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31">
@@ -51704,7 +51704,7 @@
         <v>26</v>
       </c>
       <c r="G31" t="n">
-        <v>47</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32">
@@ -51724,7 +51724,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="n">
-        <v>84</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33">
@@ -51744,7 +51744,7 @@
         <v>15</v>
       </c>
       <c r="G33" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
@@ -51764,7 +51764,7 @@
         <v>108</v>
       </c>
       <c r="G34" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -51784,7 +51784,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36">
@@ -51804,7 +51804,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -51824,7 +51824,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -58850,7 +58850,7 @@
         <v>7.8</v>
       </c>
       <c r="G2" t="n">
-        <v>5.9</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="4">
@@ -58877,7 +58877,7 @@
         <v>38.86</v>
       </c>
       <c r="G5" t="n">
-        <v>26.68</v>
+        <v>22.07</v>
       </c>
     </row>
   </sheetData>
@@ -58923,7 +58923,7 @@
         <v>4.75</v>
       </c>
       <c r="G2" t="n">
-        <v>3.905</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="4">
@@ -58950,7 +58950,7 @@
         <v>39.08</v>
       </c>
       <c r="G5" t="n">
-        <v>39.0275</v>
+        <v>37.625</v>
       </c>
     </row>
     <row r="7">
@@ -58977,7 +58977,7 @@
         <v>3.07</v>
       </c>
       <c r="G8" t="n">
-        <v>1.605909445353559</v>
+        <v>1.264050604178162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>